<commit_message>
g11.7 - correção na filtragem de tabela do siconfi
</commit_message>
<xml_diff>
--- a/Data/g11.7.xlsx
+++ b/Data/g11.7.xlsx
@@ -460,13 +460,13 @@
         <v>2017</v>
       </c>
       <c r="B2" t="n">
-        <v>-1054.253414198498</v>
+        <v>-503.9157522584894</v>
       </c>
       <c r="C2" t="n">
-        <v>-589.911135146517</v>
+        <v>-184.3024599460749</v>
       </c>
       <c r="D2" t="n">
-        <v>-1102.954904772692</v>
+        <v>-771.4996365605837</v>
       </c>
     </row>
     <row r="3">
@@ -474,13 +474,13 @@
         <v>2018</v>
       </c>
       <c r="B3" t="n">
-        <v>-1037.890765094185</v>
+        <v>-487.7016053425754</v>
       </c>
       <c r="C3" t="n">
-        <v>-664.7177760696691</v>
+        <v>-232.7429042058306</v>
       </c>
       <c r="D3" t="n">
-        <v>-1158.177848374007</v>
+        <v>-514.8661514682541</v>
       </c>
     </row>
     <row r="4">
@@ -488,13 +488,13 @@
         <v>2019</v>
       </c>
       <c r="B4" t="n">
-        <v>-1084.054438952541</v>
+        <v>-516.3149586721969</v>
       </c>
       <c r="C4" t="n">
-        <v>-733.7489607197722</v>
+        <v>-261.4772290195456</v>
       </c>
       <c r="D4" t="n">
-        <v>-1253.068240202092</v>
+        <v>-763.8795634547579</v>
       </c>
     </row>
     <row r="5">
@@ -502,13 +502,13 @@
         <v>2020</v>
       </c>
       <c r="B5" t="n">
-        <v>-1084.751953360226</v>
+        <v>-528.2070474616711</v>
       </c>
       <c r="C5" t="n">
-        <v>-746.6278737990914</v>
+        <v>-316.4916476709561</v>
       </c>
       <c r="D5" t="n">
-        <v>-1291.796819945811</v>
+        <v>-580.4121483922563</v>
       </c>
     </row>
     <row r="6">
@@ -516,10 +516,10 @@
         <v>2021</v>
       </c>
       <c r="B6" t="n">
-        <v>-355.3352083638646</v>
+        <v>-342.8572764143494</v>
       </c>
       <c r="C6" t="n">
-        <v>-222.8218619790956</v>
+        <v>-194.4217271133621</v>
       </c>
       <c r="D6" t="n">
         <v>-268.5618721834991</v>
@@ -530,10 +530,10 @@
         <v>2022</v>
       </c>
       <c r="B7" t="n">
-        <v>-350.1448687894891</v>
+        <v>-357.4461201988151</v>
       </c>
       <c r="C7" t="n">
-        <v>-221.3036524134676</v>
+        <v>-215.9024927842444</v>
       </c>
       <c r="D7" t="n">
         <v>-398.5925973798795</v>
@@ -544,10 +544,10 @@
         <v>2023</v>
       </c>
       <c r="B8" t="n">
-        <v>-372.3015922201779</v>
+        <v>-370.5427410574931</v>
       </c>
       <c r="C8" t="n">
-        <v>-234.1529161430527</v>
+        <v>-215.6927621177635</v>
       </c>
       <c r="D8" t="n">
         <v>-533.5325266161339</v>
@@ -558,10 +558,10 @@
         <v>2024</v>
       </c>
       <c r="B9" t="n">
-        <v>-385.7103366713882</v>
+        <v>-404.1582977226919</v>
       </c>
       <c r="C9" t="n">
-        <v>-239.697851680816</v>
+        <v>-232.4997573667561</v>
       </c>
       <c r="D9" t="n">
         <v>-604.477723338306</v>

</xml_diff>